<commit_message>
Macroeconomic indicators added to data
I added some more columns with some macroeconomic indicators for France
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MikkelAndersen/Library/CloudStorage/OneDrive-Aarhusuniversitet/Uni/7. semester/Business Economic and Financial Data/befd_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBCB735-F2FD-CA4A-8FF2-2F2E78DCB944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D8D8C-3553-2245-9FFD-AF0A47961AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11440" yWindow="500" windowWidth="14160" windowHeight="13780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>cons_france_volume</t>
-  </si>
-  <si>
-    <t>gdp_france_value</t>
   </si>
   <si>
     <t>prod_france_volume</t>
@@ -64,13 +61,30 @@
   <si>
     <t>NaN</t>
   </si>
+  <si>
+    <t>gdp_france_value_dollars</t>
+  </si>
+  <si>
+    <t>real_gdp_france_value_euros</t>
+  </si>
+  <si>
+    <t>total_exp_france_dollars</t>
+  </si>
+  <si>
+    <t>population_france</t>
+  </si>
+  <si>
+    <t>unemployment_france</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -78,18 +92,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Georgia"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,6 +110,17 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Georgia"/>
       <family val="1"/>
     </font>
@@ -142,31 +155,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -386,9 +400,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -396,855 +412,1289 @@
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B2" s="5">
+        <v>227425</v>
+      </c>
+      <c r="C2" s="5">
+        <v>36515</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1601090000000</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1524841.7733727</v>
+      </c>
+      <c r="F2" s="5">
+        <v>54354</v>
+      </c>
+      <c r="G2" s="5">
+        <v>55702</v>
+      </c>
+      <c r="H2" s="5">
+        <v>20876</v>
+      </c>
+      <c r="I2" s="5">
+        <v>11478</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1995</v>
-      </c>
-      <c r="B2" s="7">
-        <v>227425</v>
-      </c>
-      <c r="C2" s="7">
-        <v>36515</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1601090000000</v>
-      </c>
-      <c r="E2" s="7">
-        <v>54354</v>
-      </c>
-      <c r="F2" s="7">
-        <v>55702</v>
-      </c>
-      <c r="G2" s="7">
-        <v>20876</v>
-      </c>
-      <c r="H2" s="7">
-        <v>11478</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="K2" s="9">
+        <v>304082991822.31097</v>
+      </c>
+      <c r="L2" s="11">
+        <v>59543659</v>
+      </c>
+      <c r="M2" s="12">
+        <v>10.043011335127799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1996</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>221646</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>34795</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>1605680000000</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
+        <v>1546387.6913781001</v>
+      </c>
+      <c r="F3" s="5">
         <v>57047</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="5">
         <v>58772</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="5">
         <v>31000</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="5">
         <v>12990</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="J3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="9">
+        <v>307501028227.57996</v>
+      </c>
+      <c r="L3" s="11">
+        <v>59756533</v>
+      </c>
+      <c r="M3" s="12">
+        <v>10.558976728727099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>1997</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>225138</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>35500</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>1452880000000</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="9">
+        <v>1582515.8928725999</v>
+      </c>
+      <c r="F4" s="5">
         <v>53561</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="5">
         <v>50894</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="5">
         <v>33218</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="5">
         <v>15737</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="J4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="9">
+        <v>300796664054.242</v>
+      </c>
+      <c r="L4" s="11">
+        <v>59969944</v>
+      </c>
+      <c r="M4" s="12">
+        <v>10.7151420526513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>1998</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>228321</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>36330</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>1500000000000</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
+        <v>1639306.9987836999</v>
+      </c>
+      <c r="F5" s="5">
         <v>52671</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="5">
         <v>54188</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="5">
         <v>31175</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="5">
         <v>16485</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="J5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="9">
+        <v>318783879658.146</v>
+      </c>
+      <c r="L5" s="11">
+        <v>60192790</v>
+      </c>
+      <c r="M5" s="12">
+        <v>10.2864079027275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>1999</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>225747</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>35400</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>1490000000000</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="9">
+        <v>1695393.8192395</v>
+      </c>
+      <c r="F6" s="5">
         <v>60535</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="5">
         <v>56454</v>
       </c>
-      <c r="G6" s="7">
+      <c r="H6" s="5">
         <v>33723</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="5">
         <v>16105</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="J6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="9">
+        <v>322766419015.79095</v>
+      </c>
+      <c r="L6" s="11">
+        <v>60504420</v>
+      </c>
+      <c r="M6" s="12">
+        <v>9.9846988433823203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>2000</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>225741</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>34500</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>1370000000000</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="9">
+        <v>1761915.4643915</v>
+      </c>
+      <c r="F7" s="5">
         <v>57541</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="5">
         <v>51620</v>
       </c>
-      <c r="G7" s="7">
+      <c r="H7" s="5">
         <v>41692</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="5">
         <v>15039</v>
       </c>
-      <c r="I7" s="9">
+      <c r="J7" s="7">
         <v>5490000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="K7" s="9">
+        <v>327424014096.401</v>
+      </c>
+      <c r="L7" s="11">
+        <v>60921384</v>
+      </c>
+      <c r="M7" s="12">
+        <v>8.5274105337819908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>2001</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>227645</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>33919</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>1380000000000</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="9">
+        <v>1796866.9584995999</v>
+      </c>
+      <c r="F8" s="5">
         <v>53389</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="5">
         <v>49865</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="5">
         <v>30500</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="5">
         <v>15126</v>
       </c>
-      <c r="I8" s="9">
+      <c r="J8" s="7">
         <v>5350000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="K8" s="9">
+        <v>324707468131.49799</v>
+      </c>
+      <c r="L8" s="11">
+        <v>61367388</v>
+      </c>
+      <c r="M8" s="12">
+        <v>7.7416950519811696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>2002</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>230038</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>34820</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>1500000000000</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="9">
+        <v>1817270.9486473</v>
+      </c>
+      <c r="F9" s="5">
         <v>50353</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="5">
         <v>42507</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="5">
         <v>33478</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="5">
         <v>15541</v>
       </c>
-      <c r="I9" s="9">
+      <c r="J9" s="7">
         <v>5750000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="K9" s="9">
+        <v>332456162749.35004</v>
+      </c>
+      <c r="L9" s="11">
+        <v>61816234</v>
+      </c>
+      <c r="M9" s="12">
+        <v>7.8792318995973396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>2003</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>238947</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>34081</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>1840000000000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="9">
+        <v>1832230.0103636</v>
+      </c>
+      <c r="F10" s="5">
         <v>46360</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="5">
         <v>41807</v>
       </c>
-      <c r="G10" s="7">
+      <c r="H10" s="5">
         <v>41843</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="5">
         <v>15148</v>
       </c>
-      <c r="I10" s="9">
+      <c r="J10" s="7">
         <v>5880000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="K10" s="9">
+        <v>393594052387.60199</v>
+      </c>
+      <c r="L10" s="11">
+        <v>62256970</v>
+      </c>
+      <c r="M10" s="12">
+        <v>8.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>2004</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>238106</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>33218</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>2120000000000</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="9">
+        <v>1884077.5927148</v>
+      </c>
+      <c r="F11" s="5">
         <v>57386</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="5">
         <v>49935</v>
       </c>
-      <c r="G11" s="7">
+      <c r="H11" s="5">
         <v>42988</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="5">
         <v>14210</v>
       </c>
-      <c r="I11" s="9">
+      <c r="J11" s="7">
         <v>5590000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="K11" s="9">
+        <v>447935304055.95502</v>
+      </c>
+      <c r="L11" s="11">
+        <v>62716306</v>
+      </c>
+      <c r="M11" s="12">
+        <v>8.4749999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>2005</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>239356</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>33530</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>2200000000000</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="9">
+        <v>1915413.9480381999</v>
+      </c>
+      <c r="F12" s="5">
         <v>52105</v>
       </c>
-      <c r="F12" s="7">
+      <c r="G12" s="5">
         <v>50566</v>
       </c>
-      <c r="G12" s="7">
+      <c r="H12" s="5">
         <v>36158</v>
       </c>
-      <c r="H12" s="7">
+      <c r="I12" s="5">
         <v>13834</v>
       </c>
-      <c r="I12" s="9">
+      <c r="J12" s="7">
         <v>5670000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="K12" s="9">
+        <v>461741445446.875</v>
+      </c>
+      <c r="L12" s="11">
+        <v>63188395</v>
+      </c>
+      <c r="M12" s="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>2006</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>242595</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>33003</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>2320000000000</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="9">
+        <v>1962328.6339077</v>
+      </c>
+      <c r="F13" s="5">
         <v>52127</v>
       </c>
-      <c r="F13" s="7">
+      <c r="G13" s="5">
         <v>52036</v>
       </c>
-      <c r="G13" s="7">
+      <c r="H13" s="5">
         <v>38273</v>
       </c>
-      <c r="H13" s="7">
+      <c r="I13" s="5">
         <v>14861</v>
       </c>
-      <c r="I13" s="9">
+      <c r="J13" s="7">
         <v>6290000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="K13" s="9">
+        <v>497270615683.138</v>
+      </c>
+      <c r="L13" s="11">
+        <v>63628261</v>
+      </c>
+      <c r="M13" s="12">
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>2007</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>250096</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>32168</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>2660000000000</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="9">
+        <v>2009909.9274098</v>
+      </c>
+      <c r="F14" s="5">
         <v>45672</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="5">
         <v>45981</v>
       </c>
-      <c r="G14" s="7">
+      <c r="H14" s="5">
         <v>36408</v>
       </c>
-      <c r="H14" s="7">
+      <c r="I14" s="5">
         <v>14506</v>
       </c>
-      <c r="I14" s="9">
+      <c r="J14" s="7">
         <v>6820000000</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="K14" s="9">
+        <v>561485444728.6521</v>
+      </c>
+      <c r="L14" s="11">
+        <v>64021737</v>
+      </c>
+      <c r="M14" s="12">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>2008</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>247362</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>30800</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>2930000000000</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="9">
+        <v>2015034.1112992</v>
+      </c>
+      <c r="F15" s="5">
         <v>42654</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="5">
         <v>46970</v>
       </c>
-      <c r="G15" s="7">
+      <c r="H15" s="5">
         <v>35913</v>
       </c>
-      <c r="H15" s="7">
+      <c r="I15" s="5">
         <v>12798</v>
       </c>
-      <c r="I15" s="9">
+      <c r="J15" s="7">
         <v>6850000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="K15" s="9">
+        <v>615155181647.98596</v>
+      </c>
+      <c r="L15" s="11">
+        <v>64379696</v>
+      </c>
+      <c r="M15" s="12">
+        <v>7.0750000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>2009</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>241975</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>30214</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>2700000000000</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="9">
+        <v>1957135.8570590001</v>
+      </c>
+      <c r="F16" s="5">
         <v>46269</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="5">
         <v>47314</v>
       </c>
-      <c r="G16" s="7">
+      <c r="H16" s="5">
         <v>36093</v>
       </c>
-      <c r="H16" s="7">
+      <c r="I16" s="5">
         <v>12969</v>
       </c>
-      <c r="I16" s="9">
+      <c r="J16" s="7">
         <v>5550000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="K16" s="9">
+        <v>485607883221.297</v>
+      </c>
+      <c r="L16" s="11">
+        <v>64710879</v>
+      </c>
+      <c r="M16" s="12">
+        <v>8.7249999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>2010</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>240280</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>29272</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>2650000000000</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="9">
+        <v>1995289</v>
+      </c>
+      <c r="F17" s="5">
         <v>44381</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="5">
         <v>48525</v>
       </c>
-      <c r="G17" s="7">
+      <c r="H17" s="5">
         <v>35353</v>
       </c>
-      <c r="H17" s="7">
+      <c r="I17" s="5">
         <v>13888</v>
       </c>
-      <c r="I17" s="9">
+      <c r="J17" s="7">
         <v>6350000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="K17" s="9">
+        <v>520440953045.94397</v>
+      </c>
+      <c r="L17" s="11">
+        <v>65030575</v>
+      </c>
+      <c r="M17" s="12">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>2011</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>242191</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>28307</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>2870000000000</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="9">
+        <v>2039039.7148593001</v>
+      </c>
+      <c r="F18" s="5">
         <v>50757</v>
       </c>
-      <c r="F18" s="7">
+      <c r="G18" s="5">
         <v>42772</v>
       </c>
-      <c r="G18" s="7">
+      <c r="H18" s="5">
         <v>33397</v>
       </c>
-      <c r="H18" s="7">
+      <c r="I18" s="5">
         <v>14722</v>
       </c>
-      <c r="I18" s="9">
+      <c r="J18" s="7">
         <v>7200000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+      <c r="K18" s="9">
+        <v>594734227974.13</v>
+      </c>
+      <c r="L18" s="11">
+        <v>65345233</v>
+      </c>
+      <c r="M18" s="12">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>2012</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>244620</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>28022</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>2680000000000</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="9">
+        <v>2045424.6566627</v>
+      </c>
+      <c r="F19" s="5">
         <v>41548</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="5">
         <v>45616</v>
       </c>
-      <c r="G19" s="7">
+      <c r="H19" s="5">
         <v>31123</v>
       </c>
-      <c r="H19" s="7">
+      <c r="I19" s="5">
         <v>15006</v>
       </c>
-      <c r="I19" s="9">
+      <c r="J19" s="7">
         <v>7860000000</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="K19" s="9">
+        <v>569345270862.92493</v>
+      </c>
+      <c r="L19" s="11">
+        <v>65662240</v>
+      </c>
+      <c r="M19" s="12">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>2013</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>244433</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>27770</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <v>2810000000000</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="9">
+        <v>2057212.9846826999</v>
+      </c>
+      <c r="F20" s="5">
         <v>42134</v>
       </c>
-      <c r="F20" s="7">
+      <c r="G20" s="5">
         <v>54029</v>
       </c>
-      <c r="G20" s="7">
+      <c r="H20" s="5">
         <v>45308</v>
       </c>
-      <c r="H20" s="7">
+      <c r="I20" s="5">
         <v>14532</v>
       </c>
-      <c r="I20" s="9">
+      <c r="J20" s="7">
         <v>7840000000</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+      <c r="K20" s="9">
+        <v>581415603025.35901</v>
+      </c>
+      <c r="L20" s="11">
+        <v>66002289</v>
+      </c>
+      <c r="M20" s="12">
+        <v>9.9250000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>2014</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>239089</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>27545</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>2860000000000</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="9">
+        <v>2076883.7064344001</v>
+      </c>
+      <c r="F21" s="5">
         <v>46534</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="5">
         <v>44229</v>
       </c>
-      <c r="G21" s="7">
+      <c r="H21" s="5">
         <v>39494</v>
       </c>
-      <c r="H21" s="7">
+      <c r="I21" s="5">
         <v>14307</v>
       </c>
-      <c r="I21" s="9">
+      <c r="J21" s="7">
         <v>7750000000</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="K21" s="9">
+        <v>583627098049.40796</v>
+      </c>
+      <c r="L21" s="11">
+        <v>66312067</v>
+      </c>
+      <c r="M21" s="12">
+        <v>10.324999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>2015</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>241418</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>26452</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <v>2440000000000</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="9">
+        <v>2099997.6015237002</v>
+      </c>
+      <c r="F22" s="5">
         <v>47775</v>
       </c>
-      <c r="F22" s="7">
+      <c r="G22" s="5">
         <v>49996</v>
       </c>
-      <c r="G22" s="7">
+      <c r="H22" s="5">
         <v>37703</v>
       </c>
-      <c r="H22" s="7">
+      <c r="I22" s="5">
         <v>13982</v>
       </c>
-      <c r="I22" s="9">
+      <c r="J22" s="7">
         <v>8279999999.999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
+      <c r="K22" s="9">
+        <v>506843014046.47699</v>
+      </c>
+      <c r="L22" s="11">
+        <v>66548272</v>
+      </c>
+      <c r="M22" s="12">
+        <v>10.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>2016</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>244630</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>28290</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>2470000000000</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
+        <v>2123002.3275367999</v>
+      </c>
+      <c r="F23" s="5">
         <v>45367</v>
       </c>
-      <c r="F23" s="7">
+      <c r="G23" s="5">
         <v>50920</v>
       </c>
-      <c r="G23" s="7">
+      <c r="H23" s="5">
         <v>39970</v>
       </c>
-      <c r="H23" s="7">
+      <c r="I23" s="5">
         <v>14539</v>
       </c>
-      <c r="I23" s="9">
+      <c r="J23" s="7">
         <v>8289999999.999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+      <c r="K23" s="9">
+        <v>499196445417.23499</v>
+      </c>
+      <c r="L23" s="11">
+        <v>66724104</v>
+      </c>
+      <c r="M23" s="12">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>2017</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>246189</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <v>28634</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>2600000000000</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="9">
+        <v>2171649.2271532002</v>
+      </c>
+      <c r="F24" s="5">
         <v>36605</v>
       </c>
-      <c r="F24" s="7">
+      <c r="G24" s="5">
         <v>42500</v>
       </c>
-      <c r="G24" s="7">
+      <c r="H24" s="5">
         <v>32480</v>
       </c>
-      <c r="H24" s="7">
+      <c r="I24" s="5">
         <v>14821</v>
       </c>
-      <c r="I24" s="9">
+      <c r="J24" s="7">
         <v>9110000000</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+      <c r="K24" s="9">
+        <v>536726659480.64606</v>
+      </c>
+      <c r="L24" s="11">
+        <v>66918020</v>
+      </c>
+      <c r="M24" s="12">
+        <v>9.4250000000000007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>2018</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>241062</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>26028</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>2790000000000</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="9">
+        <v>2212151.9204747998</v>
+      </c>
+      <c r="F25" s="5">
         <v>49186</v>
       </c>
-      <c r="F25" s="7">
+      <c r="G25" s="5">
         <v>54783</v>
       </c>
-      <c r="G25" s="7">
+      <c r="H25" s="5">
         <v>44933</v>
       </c>
-      <c r="H25" s="7">
+      <c r="I25" s="5">
         <v>14188</v>
       </c>
-      <c r="I25" s="9">
+      <c r="J25" s="7">
         <v>9370000000</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+      <c r="K25" s="9">
+        <v>582825380447.85303</v>
+      </c>
+      <c r="L25" s="11">
+        <v>67158348</v>
+      </c>
+      <c r="M25" s="12">
+        <v>9.0250000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>2019</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>236672</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>24714</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>2730000000000</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="9">
+        <v>2252921.2568494999</v>
+      </c>
+      <c r="F26" s="5">
         <v>42324</v>
       </c>
-      <c r="F26" s="7">
+      <c r="G26" s="5">
         <v>47533</v>
       </c>
-      <c r="G26" s="7">
+      <c r="H26" s="5">
         <v>33676</v>
       </c>
-      <c r="H26" s="7">
+      <c r="I26" s="5">
         <v>13517</v>
       </c>
-      <c r="I26" s="9">
+      <c r="J26" s="7">
         <v>9800000000</v>
       </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+      <c r="K26" s="9">
+        <v>572063356708.39905</v>
+      </c>
+      <c r="L26" s="11">
+        <v>67388001</v>
+      </c>
+      <c r="M26" s="12">
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>2020</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>231414</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <v>24361</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>2640000000000</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="9">
+        <v>2083040.6491054001</v>
+      </c>
+      <c r="F27" s="5">
         <v>46739</v>
       </c>
-      <c r="F27" s="7">
+      <c r="G27" s="5">
         <v>49066</v>
       </c>
-      <c r="G27" s="7">
+      <c r="H27" s="5">
         <v>40949</v>
       </c>
-      <c r="H27" s="7">
+      <c r="I27" s="5">
         <v>14085</v>
       </c>
-      <c r="I27" s="9">
+      <c r="J27" s="7">
         <v>8740000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+      <c r="K27" s="9">
+        <v>487187033185.53296</v>
+      </c>
+      <c r="L27" s="11">
+        <v>67571107</v>
+      </c>
+      <c r="M27" s="12">
+        <v>8.0250000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>2021</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>234033</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>23228</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>2960000000000</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="9">
+        <v>2217088.6813486</v>
+      </c>
+      <c r="F28" s="5">
         <v>37753</v>
       </c>
-      <c r="F28" s="7">
+      <c r="G28" s="5">
         <v>50232</v>
       </c>
-      <c r="G28" s="7">
+      <c r="H28" s="5">
         <v>35471</v>
       </c>
-      <c r="H28" s="7">
+      <c r="I28" s="5">
         <v>15163</v>
       </c>
-      <c r="I28" s="9">
+      <c r="J28" s="7">
         <v>11100000000</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+      <c r="K28" s="9">
+        <v>582209198742.22998</v>
+      </c>
+      <c r="L28" s="11">
+        <v>67749632</v>
+      </c>
+      <c r="M28" s="12">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>2022</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>231600</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>24872</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>2780000000000</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="9">
+        <v>2271512.8471146999</v>
+      </c>
+      <c r="F29" s="5">
         <v>45616</v>
       </c>
-      <c r="F29" s="7">
+      <c r="G29" s="5">
         <v>49843</v>
       </c>
-      <c r="G29" s="7">
+      <c r="H29" s="5">
         <v>35703</v>
       </c>
-      <c r="H29" s="7">
+      <c r="I29" s="5">
         <v>14453</v>
       </c>
-      <c r="I29" s="9">
+      <c r="J29" s="7">
         <v>12280000000</v>
       </c>
-      <c r="K29" s="2"/>
+      <c r="K29" s="9">
+        <v>616478436577.146</v>
+      </c>
+      <c r="L29" s="11">
+        <v>67935660</v>
+      </c>
+      <c r="M29" s="12">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C59" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>